<commit_message>
Better support on excel file; Extract labels in x-layout
</commit_message>
<xml_diff>
--- a/app/test.xlsx
+++ b/app/test.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Milk\Projects\heatgraphy\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{191A0C27-22D6-47F8-B248-56AF384C412E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66B0A2EC-45D2-45AC-B705-6209EF705153}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13340" yWindow="3690" windowWidth="21570" windowHeight="14980" xr2:uid="{62C9015D-B0D6-4571-8C01-D6231DDCBE04}"/>
+    <workbookView xWindow="13340" yWindow="3690" windowWidth="21570" windowHeight="14980" activeTab="1" xr2:uid="{62C9015D-B0D6-4571-8C01-D6231DDCBE04}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,6 +34,32 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -374,7 +401,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -384,8 +411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17C45EDA-D6D4-4470-87AD-F3DE33BC95A0}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -463,4 +490,135 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB69B22E-D1E5-448D-8A8E-EE40D78E3FDA}">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix excel parsing error
</commit_message>
<xml_diff>
--- a/app/test.xlsx
+++ b/app/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Milk\Projects\heatgraphy\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C88AF059-DCB5-4A66-83B0-44F87C01A0E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB2C0895-F75E-45A8-87CF-B8DB1D8C79AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9700" yWindow="3990" windowWidth="21570" windowHeight="14980" activeTab="1" xr2:uid="{62C9015D-B0D6-4571-8C01-D6231DDCBE04}"/>
+    <workbookView xWindow="14500" yWindow="4000" windowWidth="21570" windowHeight="14980" activeTab="1" xr2:uid="{62C9015D-B0D6-4571-8C01-D6231DDCBE04}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
   <si>
     <t>a</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>g</t>
+  </si>
+  <si>
+    <t>c</t>
   </si>
 </sst>
 </file>
@@ -494,7 +497,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -507,7 +510,7 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>

</xml_diff>